<commit_message>
Example template can be downloaded as ods as well as xlsx.
</commit_message>
<xml_diff>
--- a/example_data/ShinyABCi_data_template.xlsx
+++ b/example_data/ShinyABCi_data_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment A" sheetId="1" state="visible" r:id="rId2"/>
@@ -134,7 +134,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -156,26 +156,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -203,7 +183,7 @@
   </sheetPr>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -515,27 +495,27 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
-      <c r="B19" s="6"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
-      <c r="B20" s="6"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
@@ -821,14 +801,14 @@
   </sheetPr>
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1167,182 +1147,178 @@
         <v>8</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
-      <c r="B22" s="6"/>
+      <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
-      <c r="B23" s="6"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
-      <c r="B24" s="6"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
       <c r="K27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
       <c r="K28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
       <c r="K29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
       <c r="K30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
       <c r="K31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
       <c r="K32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
+      <c r="B34" s="1"/>
+      <c r="D34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="10"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="7"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -1352,10 +1328,10 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="7"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -1365,10 +1341,9 @@
       <c r="K37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="7"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>

</xml_diff>